<commit_message>
Update template import voucher code
</commit_message>
<xml_diff>
--- a/IMP/IMP.WebApi/App_Datas/ExcelTemplates/import_voucher_code_template.xlsx
+++ b/IMP/IMP.WebApi/App_Datas/ExcelTemplates/import_voucher_code_template.xlsx
@@ -1,152 +1,240 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhtha\AppData\Local\Temp\MicrosoftEdgeDownloads\08394e90-071f-41a3-ace2-1038ef4bfa92\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF50DC1E-DCDC-47DB-9641-C056DF70B98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Danh sách Voucher" sheetId="1" r:id="rId1"/>
+    <sheet name="Ref" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>ABCDS</t>
-  </si>
-  <si>
-    <t>AKABIO</t>
-  </si>
-  <si>
-    <t>ATKBON</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Hình thức giảm</t>
+  </si>
+  <si>
+    <t>Mức cố định</t>
+  </si>
+  <si>
+    <t>Theo phần trăm</t>
+  </si>
+  <si>
+    <t>Miễn phí giao hàng</t>
+  </si>
+  <si>
+    <t>Số lần sử dụng (tối đa 10.000)</t>
+  </si>
+  <si>
+    <t>Mã Voucher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
-    <font/>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="1">
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -287,52 +375,87 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25" style="3" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+    <row r="1" spans="1:2" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>100.0</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>0</formula1>
+      <formula2>10000</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>